<commit_message>
updated tex and main pdf, figures, and old versions
</commit_message>
<xml_diff>
--- a/text/word_count.xlsx
+++ b/text/word_count.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41203800_oneimpact\cumulative_influence_paper\text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41203800_oneimpact\cumulative_zoi_paper\text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D0DBCA-B742-4582-B691-D3DC9573FAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF075D7-2649-42F1-ACEC-8AD63B396797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{7037B53F-4623-4F2F-961B-2A6A3BCFCAB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7037B53F-4623-4F2F-961B-2A6A3BCFCAB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Abstract</t>
   </si>
@@ -72,10 +72,31 @@
     <t>total:</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Max allowed: 7000</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2_after_bram_review</t>
+  </si>
+  <si>
+    <t>Max abstract: 350</t>
+  </si>
+  <si>
+    <t>Title page</t>
+  </si>
+  <si>
+    <t>v3_before_Manu</t>
+  </si>
+  <si>
+    <t>Estimating</t>
+  </si>
+  <si>
+    <t>v4_after_Manu</t>
+  </si>
+  <si>
+    <t>v5_after_Audun</t>
   </si>
 </sst>
 </file>
@@ -427,122 +448,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E74D4F-A22F-4768-9391-F90CC184B98D}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>98</v>
+      </c>
+      <c r="D2">
+        <v>111</v>
+      </c>
+      <c r="E2">
+        <v>105</v>
+      </c>
+      <c r="F2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B3">
         <v>342</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C3">
+        <v>358</v>
+      </c>
+      <c r="D3">
+        <v>352</v>
+      </c>
+      <c r="E3">
+        <v>372</v>
+      </c>
+      <c r="F3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B4">
         <v>1400</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C4">
+        <v>1039</v>
+      </c>
+      <c r="D4">
+        <v>1125</v>
+      </c>
+      <c r="E4">
+        <v>1110</v>
+      </c>
+      <c r="F4">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>425</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C5">
+        <v>434</v>
+      </c>
+      <c r="D5">
+        <v>531</v>
+      </c>
+      <c r="E5">
+        <v>502</v>
+      </c>
+      <c r="F5">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>960</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="C6">
+        <v>825</v>
+      </c>
+      <c r="D6">
+        <v>958</v>
+      </c>
+      <c r="E6">
+        <v>1023</v>
+      </c>
+      <c r="F6">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>207</v>
+      </c>
+      <c r="E7">
+        <v>226</v>
+      </c>
+      <c r="F7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>500</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C8">
+        <v>535</v>
+      </c>
+      <c r="D8">
+        <v>463</v>
+      </c>
+      <c r="E8">
+        <v>429</v>
+      </c>
+      <c r="F8">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>1094</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C9">
+        <v>1040</v>
+      </c>
+      <c r="D9">
+        <v>995</v>
+      </c>
+      <c r="E9">
+        <v>952</v>
+      </c>
+      <c r="F9">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>270</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>1928</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C11">
+        <v>1714</v>
+      </c>
+      <c r="D11">
+        <v>1643</v>
+      </c>
+      <c r="E11">
+        <v>1570</v>
+      </c>
+      <c r="F11">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>232</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C12">
+        <v>140</v>
+      </c>
+      <c r="D12">
+        <v>282</v>
+      </c>
+      <c r="E12">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>1923</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C13">
+        <v>1239</v>
+      </c>
+      <c r="D13">
+        <v>1250</v>
+      </c>
+      <c r="E13">
+        <v>1297</v>
+      </c>
+      <c r="F13">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <v>529</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="C14">
+        <v>428</v>
+      </c>
+      <c r="D14">
+        <v>473</v>
+      </c>
+      <c r="E14">
+        <f>134+76+119+80+51</f>
+        <v>460</v>
+      </c>
+      <c r="F14">
+        <f>134+76+119+80+51</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <f>SUM(B1:B11)</f>
-        <v>9603</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B16">
+        <f t="shared" ref="B16:C16" si="0">SUM(B2:B11,B13:B14)</f>
+        <v>9371</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>7710</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D2:D11,D13:D14)</f>
+        <v>8108</v>
+      </c>
+      <c r="E16">
+        <f>SUM(E2:E11,E13:E14)</f>
+        <v>8046</v>
+      </c>
+      <c r="F16">
+        <f>SUM(F2:F11,F13:F14)</f>
+        <v>7749</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>13</v>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>